<commit_message>
rerun corona results with larger ds
</commit_message>
<xml_diff>
--- a/results/mp/tinybert/corona/confidence/126/0.1/avg_0.002_scores.xlsx
+++ b/results/mp/tinybert/corona/confidence/126/0.1/avg_0.002_scores.xlsx
@@ -40,235 +40,235 @@
     <t>name</t>
   </si>
   <si>
+    <t>killed</t>
+  </si>
+  <si>
     <t>arrested</t>
   </si>
   <si>
-    <t>accused</t>
-  </si>
-  <si>
-    <t>killed</t>
-  </si>
-  <si>
     <t>crude</t>
   </si>
   <si>
+    <t>died</t>
+  </si>
+  <si>
+    <t>fraud</t>
+  </si>
+  <si>
+    <t>crisis</t>
+  </si>
+  <si>
     <t>forced</t>
   </si>
   <si>
-    <t>fraud</t>
-  </si>
-  <si>
-    <t>crisis</t>
-  </si>
-  <si>
-    <t>died</t>
-  </si>
-  <si>
     <t>warning</t>
   </si>
   <si>
     <t>war</t>
   </si>
   <si>
+    <t>panic</t>
+  </si>
+  <si>
     <t>emergency</t>
   </si>
   <si>
-    <t>panic</t>
-  </si>
-  <si>
-    <t>fears</t>
-  </si>
-  <si>
     <t>sc</t>
   </si>
   <si>
     <t>low</t>
   </si>
   <si>
+    <t>stop</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
-    <t>stop</t>
-  </si>
-  <si>
     <t>negative</t>
   </si>
   <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>beauty</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>interesting</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>friend</t>
+  </si>
+  <si>
+    <t>amazing</t>
+  </si>
+  <si>
+    <t>great</t>
+  </si>
+  <si>
+    <t>love</t>
+  </si>
+  <si>
+    <t>wow</t>
+  </si>
+  <si>
+    <t>nice</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>thanks</t>
+  </si>
+  <si>
     <t>won</t>
   </si>
   <si>
-    <t>amazing</t>
-  </si>
-  <si>
-    <t>friend</t>
-  </si>
-  <si>
-    <t>enjoy</t>
-  </si>
-  <si>
-    <t>love</t>
-  </si>
-  <si>
-    <t>interesting</t>
-  </si>
-  <si>
-    <t>best</t>
-  </si>
-  <si>
-    <t>happy</t>
-  </si>
-  <si>
-    <t>thanks</t>
-  </si>
-  <si>
-    <t>wow</t>
-  </si>
-  <si>
-    <t>creative</t>
-  </si>
-  <si>
-    <t>strong</t>
-  </si>
-  <si>
-    <t>great</t>
-  </si>
-  <si>
     <t>thank</t>
   </si>
   <si>
+    <t>friends</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
     <t>free</t>
   </si>
   <si>
-    <t>positive</t>
-  </si>
-  <si>
-    <t>brilliant</t>
-  </si>
-  <si>
-    <t>nice</t>
+    <t>support</t>
+  </si>
+  <si>
+    <t>safe</t>
+  </si>
+  <si>
+    <t>ensure</t>
+  </si>
+  <si>
+    <t>safety</t>
   </si>
   <si>
     <t>confidence</t>
   </si>
   <si>
-    <t>support</t>
-  </si>
-  <si>
-    <t>fun</t>
+    <t>good</t>
+  </si>
+  <si>
+    <t>heroes</t>
+  </si>
+  <si>
+    <t>boost</t>
   </si>
   <si>
     <t>healthy</t>
   </si>
   <si>
-    <t>boost</t>
-  </si>
-  <si>
-    <t>safety</t>
-  </si>
-  <si>
-    <t>heroes</t>
-  </si>
-  <si>
-    <t>ensure</t>
-  </si>
-  <si>
     <t>well</t>
   </si>
   <si>
-    <t>safe</t>
-  </si>
-  <si>
-    <t>effective</t>
-  </si>
-  <si>
-    <t>sharing</t>
-  </si>
-  <si>
     <t>fresh</t>
   </si>
   <si>
-    <t>friends</t>
-  </si>
-  <si>
-    <t>special</t>
+    <t>better</t>
   </si>
   <si>
     <t>relief</t>
   </si>
   <si>
-    <t>better</t>
-  </si>
-  <si>
-    <t>good</t>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>important</t>
   </si>
   <si>
     <t>credit</t>
   </si>
   <si>
-    <t>worth</t>
-  </si>
-  <si>
     <t>ready</t>
   </si>
   <si>
-    <t>hand</t>
-  </si>
-  <si>
     <t>energy</t>
   </si>
   <si>
+    <t>dear</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>care</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>giving</t>
+  </si>
+  <si>
+    <t>protect</t>
+  </si>
+  <si>
     <t>hope</t>
   </si>
   <si>
-    <t>like</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>important</t>
-  </si>
-  <si>
-    <t>help</t>
-  </si>
-  <si>
-    <t>protect</t>
-  </si>
-  <si>
-    <t>care</t>
+    <t>please</t>
+  </si>
+  <si>
+    <t>increase</t>
+  </si>
+  <si>
+    <t>sure</t>
   </si>
   <si>
     <t>join</t>
   </si>
   <si>
-    <t>please</t>
-  </si>
-  <si>
-    <t>sure</t>
-  </si>
-  <si>
-    <t>alert</t>
-  </si>
-  <si>
-    <t>increase</t>
-  </si>
-  <si>
-    <t>share</t>
-  </si>
-  <si>
     <t>$</t>
   </si>
   <si>
+    <t>you</t>
+  </si>
+  <si>
     <t>store</t>
   </si>
   <si>
-    <t>you</t>
+    <t>!</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
+    <t>co</t>
+  </si>
+  <si>
     <t>to</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -626,7 +626,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -634,10 +634,10 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -698,10 +698,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -716,16 +716,16 @@
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>26</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>12</v>
-      </c>
       <c r="M3">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -745,13 +745,13 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -763,19 +763,19 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="M4">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -795,13 +795,13 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.8823529411764706</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -813,19 +813,19 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0.9545454545454546</v>
       </c>
       <c r="L5">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="M5">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -845,13 +845,13 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.92</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="C6">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D6">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -863,31 +863,31 @@
         <v>0</v>
       </c>
       <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6">
+        <v>0.9393939393939394</v>
+      </c>
+      <c r="L6">
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <v>31</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>2</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>7</v>
-      </c>
-      <c r="M6">
-        <v>7</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -895,13 +895,13 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.9090909090909091</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -913,19 +913,19 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K7">
-        <v>0.9583333333333334</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="L7">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="M7">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -937,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -945,13 +945,13 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.7647058823529411</v>
+        <v>0.5856164383561644</v>
       </c>
       <c r="C8">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="D8">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -963,13 +963,13 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K8">
-        <v>0.9444444444444444</v>
+        <v>0.8947368421052632</v>
       </c>
       <c r="L8">
         <v>17</v>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -995,13 +995,13 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.7272727272727273</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="C9">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1013,19 +1013,19 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K9">
-        <v>0.9375</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="L9">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="M9">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1045,13 +1045,13 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.7</v>
+        <v>0.52</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1063,19 +1063,19 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K10">
-        <v>0.9090909090909091</v>
+        <v>0.8839285714285714</v>
       </c>
       <c r="L10">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="M10">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1087,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1095,13 +1095,13 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.4666666666666667</v>
+        <v>0.3421052631578947</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1113,19 +1113,19 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K11">
-        <v>0.9</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="L11">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M11">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1145,13 +1145,13 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.375</v>
+        <v>0.187984496124031</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1163,19 +1163,19 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>15</v>
+        <v>419</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K12">
-        <v>0.8888888888888888</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="L12">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M12">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1195,13 +1195,13 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.3571428571428572</v>
+        <v>0.1866666666666667</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1213,19 +1213,19 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K13">
-        <v>0.8888888888888888</v>
+        <v>0.8518518518518519</v>
       </c>
       <c r="L13">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="M13">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -1237,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1245,13 +1245,13 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.3090128755364807</v>
+        <v>0.1534391534391534</v>
       </c>
       <c r="C14">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D14">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1263,19 +1263,19 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K14">
-        <v>0.8888888888888888</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="L14">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="M14">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1295,13 +1295,13 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.2592592592592592</v>
+        <v>0.1275167785234899</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1313,19 +1313,19 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K15">
-        <v>0.8823529411764706</v>
+        <v>0.8048780487804879</v>
       </c>
       <c r="L15">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="M15">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1345,13 +1345,13 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.1976744186046512</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="C16">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D16">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1363,19 +1363,19 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>69</v>
+        <v>238</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K16">
-        <v>0.8703703703703703</v>
+        <v>0.7948717948717948</v>
       </c>
       <c r="L16">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M16">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -1387,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1395,7 +1395,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>0.1875</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="C17">
         <v>15</v>
@@ -1413,119 +1413,71 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>65</v>
+        <v>345</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17">
+        <v>0.7890625</v>
+      </c>
+      <c r="L17">
+        <v>101</v>
+      </c>
+      <c r="M17">
+        <v>101</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="J18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="L18">
+        <v>22</v>
+      </c>
+      <c r="M18">
+        <v>22</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="J19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K17">
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="L17">
-        <v>48</v>
-      </c>
-      <c r="M17">
-        <v>48</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>0.1185185185185185</v>
-      </c>
-      <c r="C18">
-        <v>16</v>
-      </c>
-      <c r="D18">
-        <v>16</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>119</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K18">
-        <v>0.8518518518518519</v>
-      </c>
-      <c r="L18">
-        <v>23</v>
-      </c>
-      <c r="M18">
-        <v>23</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>0.07272727272727272</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>102</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="K19">
-        <v>0.8181818181818182</v>
+        <v>0.7586206896551724</v>
       </c>
       <c r="L19">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="M19">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -1537,21 +1489,21 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="J20" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K20">
-        <v>0.8125</v>
+        <v>0.7416666666666667</v>
       </c>
       <c r="L20">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="M20">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -1563,21 +1515,21 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="J21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K21">
-        <v>0.8</v>
+        <v>0.7264150943396226</v>
       </c>
       <c r="L21">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="M21">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -1589,21 +1541,21 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="J22" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K22">
-        <v>0.7843137254901961</v>
+        <v>0.7253521126760564</v>
       </c>
       <c r="L22">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="M22">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -1615,47 +1567,47 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="J23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K23">
-        <v>0.7777777777777778</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="L23">
+        <v>17</v>
+      </c>
+      <c r="M23">
+        <v>17</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23">
         <v>7</v>
-      </c>
-      <c r="M23">
-        <v>7</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="J24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K24">
-        <v>0.7777777777777778</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="L24">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="M24">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -1667,21 +1619,21 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="J25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K25">
-        <v>0.7647058823529411</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="L25">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="M25">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -1693,21 +1645,21 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="J26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K26">
-        <v>0.7586206896551724</v>
+        <v>0.6875</v>
       </c>
       <c r="L26">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="M26">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -1719,21 +1671,21 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="J27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K27">
-        <v>0.75</v>
+        <v>0.6595744680851063</v>
       </c>
       <c r="L27">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="M27">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="N27">
         <v>1</v>
@@ -1745,21 +1697,21 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="J28" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K28">
-        <v>0.75</v>
+        <v>0.6521739130434783</v>
       </c>
       <c r="L28">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M28">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -1771,21 +1723,21 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="J29" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K29">
-        <v>0.7435897435897436</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="L29">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M29">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -1802,16 +1754,16 @@
     </row>
     <row r="30" spans="1:17">
       <c r="J30" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K30">
-        <v>0.7241379310344828</v>
+        <v>0.6170212765957447</v>
       </c>
       <c r="L30">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="M30">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="N30">
         <v>1</v>
@@ -1823,21 +1775,21 @@
         <v>0</v>
       </c>
       <c r="Q30">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="J31" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K31">
-        <v>0.7</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="L31">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="M31">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -1849,21 +1801,21 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="J32" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K32">
-        <v>0.7</v>
+        <v>0.6031746031746031</v>
       </c>
       <c r="L32">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="M32">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="N32">
         <v>1</v>
@@ -1875,21 +1827,21 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="10:17">
       <c r="J33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K33">
-        <v>0.6923076923076923</v>
+        <v>0.6</v>
       </c>
       <c r="L33">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="M33">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="N33">
         <v>1</v>
@@ -1901,21 +1853,21 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="10:17">
       <c r="J34" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K34">
-        <v>0.6923076923076923</v>
+        <v>0.5326370757180157</v>
       </c>
       <c r="L34">
-        <v>9</v>
+        <v>204</v>
       </c>
       <c r="M34">
-        <v>9</v>
+        <v>204</v>
       </c>
       <c r="N34">
         <v>1</v>
@@ -1927,21 +1879,21 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>4</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="10:17">
       <c r="J35" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K35">
-        <v>0.6923076923076923</v>
+        <v>0.5111111111111111</v>
       </c>
       <c r="L35">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="M35">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="N35">
         <v>1</v>
@@ -1953,15 +1905,15 @@
         <v>0</v>
       </c>
       <c r="Q35">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="10:17">
       <c r="J36" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K36">
-        <v>0.68</v>
+        <v>0.5</v>
       </c>
       <c r="L36">
         <v>17</v>
@@ -1979,21 +1931,21 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="10:17">
       <c r="J37" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K37">
-        <v>0.6666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="L37">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="M37">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="N37">
         <v>1</v>
@@ -2005,21 +1957,21 @@
         <v>0</v>
       </c>
       <c r="Q37">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="10:17">
       <c r="J38" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K38">
-        <v>0.6575342465753424</v>
+        <v>0.475</v>
       </c>
       <c r="L38">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="M38">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -2031,21 +1983,21 @@
         <v>0</v>
       </c>
       <c r="Q38">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="10:17">
       <c r="J39" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K39">
-        <v>0.631578947368421</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="L39">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M39">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N39">
         <v>1</v>
@@ -2057,21 +2009,21 @@
         <v>0</v>
       </c>
       <c r="Q39">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="10:17">
       <c r="J40" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K40">
-        <v>0.5833333333333334</v>
+        <v>0.4529411764705882</v>
       </c>
       <c r="L40">
-        <v>7</v>
+        <v>154</v>
       </c>
       <c r="M40">
-        <v>7</v>
+        <v>154</v>
       </c>
       <c r="N40">
         <v>1</v>
@@ -2083,21 +2035,21 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <v>5</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="10:17">
       <c r="J41" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K41">
-        <v>0.5714285714285714</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="L41">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M41">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N41">
         <v>1</v>
@@ -2109,21 +2061,21 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="10:17">
       <c r="J42" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K42">
-        <v>0.5446009389671361</v>
+        <v>0.4157303370786517</v>
       </c>
       <c r="L42">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="M42">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="N42">
         <v>1</v>
@@ -2135,21 +2087,21 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <v>97</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="10:17">
       <c r="J43" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K43">
-        <v>0.5</v>
+        <v>0.4067796610169492</v>
       </c>
       <c r="L43">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="M43">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="N43">
         <v>1</v>
@@ -2161,21 +2113,21 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <v>11</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="10:17">
       <c r="J44" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K44">
-        <v>0.5</v>
+        <v>0.3939393939393939</v>
       </c>
       <c r="L44">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M44">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N44">
         <v>1</v>
@@ -2187,21 +2139,21 @@
         <v>0</v>
       </c>
       <c r="Q44">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="10:17">
       <c r="J45" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K45">
-        <v>0.5</v>
+        <v>0.3698630136986301</v>
       </c>
       <c r="L45">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="M45">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="N45">
         <v>1</v>
@@ -2213,21 +2165,21 @@
         <v>0</v>
       </c>
       <c r="Q45">
-        <v>72</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="10:17">
       <c r="J46" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K46">
-        <v>0.5</v>
+        <v>0.3692307692307693</v>
       </c>
       <c r="L46">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="M46">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="N46">
         <v>1</v>
@@ -2239,21 +2191,21 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="10:17">
       <c r="J47" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K47">
-        <v>0.4705882352941176</v>
+        <v>0.3514644351464435</v>
       </c>
       <c r="L47">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="M47">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="N47">
         <v>1</v>
@@ -2265,21 +2217,21 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>9</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="10:17">
       <c r="J48" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K48">
-        <v>0.4651162790697674</v>
+        <v>0.3461538461538461</v>
       </c>
       <c r="L48">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="M48">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="N48">
         <v>1</v>
@@ -2291,21 +2243,21 @@
         <v>0</v>
       </c>
       <c r="Q48">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="10:17">
       <c r="J49" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K49">
-        <v>0.4333333333333333</v>
+        <v>0.34375</v>
       </c>
       <c r="L49">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="M49">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -2317,21 +2269,21 @@
         <v>0</v>
       </c>
       <c r="Q49">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="10:17">
       <c r="J50" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K50">
-        <v>0.4</v>
+        <v>0.3023255813953488</v>
       </c>
       <c r="L50">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M50">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N50">
         <v>1</v>
@@ -2343,21 +2295,21 @@
         <v>0</v>
       </c>
       <c r="Q50">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="10:17">
       <c r="J51" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K51">
-        <v>0.4</v>
+        <v>0.146551724137931</v>
       </c>
       <c r="L51">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M51">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -2369,21 +2321,21 @@
         <v>0</v>
       </c>
       <c r="Q51">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="10:17">
       <c r="J52" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K52">
-        <v>0.3804347826086957</v>
+        <v>0.01833333333333333</v>
       </c>
       <c r="L52">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="M52">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -2395,21 +2347,21 @@
         <v>0</v>
       </c>
       <c r="Q52">
-        <v>57</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="53" spans="10:17">
       <c r="J53" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K53">
-        <v>0.2916666666666667</v>
+        <v>0.01789709172259508</v>
       </c>
       <c r="L53">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="M53">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -2421,151 +2373,151 @@
         <v>0</v>
       </c>
       <c r="Q53">
-        <v>17</v>
+        <v>878</v>
       </c>
     </row>
     <row r="54" spans="10:17">
       <c r="J54" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K54">
-        <v>0.25</v>
+        <v>0.01317122593718338</v>
       </c>
       <c r="L54">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M54">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N54">
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="O54">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="P54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q54">
-        <v>24</v>
+        <v>974</v>
       </c>
     </row>
     <row r="55" spans="10:17">
       <c r="J55" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K55">
-        <v>0.2432432432432433</v>
+        <v>0.0101161483701761</v>
       </c>
       <c r="L55">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="M55">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="N55">
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="O55">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="P55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q55">
-        <v>28</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="56" spans="10:17">
       <c r="J56" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K56">
-        <v>0.2105263157894737</v>
+        <v>0.008165829145728644</v>
       </c>
       <c r="L56">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M56">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N56">
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="O56">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="P56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q56">
-        <v>30</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="57" spans="10:17">
       <c r="J57" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K57">
-        <v>0.1481481481481481</v>
+        <v>0.007774140752864157</v>
       </c>
       <c r="L57">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="M57">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="N57">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="O57">
-        <v>0</v>
+        <v>0.05000000000000004</v>
       </c>
       <c r="P57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q57">
-        <v>46</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="58" spans="10:17">
       <c r="J58" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K58">
-        <v>0.02439024390243903</v>
+        <v>0.00700280112044818</v>
       </c>
       <c r="L58">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="M58">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="N58">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="O58">
-        <v>0</v>
+        <v>0.06000000000000005</v>
       </c>
       <c r="P58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q58">
-        <v>400</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="59" spans="10:17">
       <c r="J59" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K59">
-        <v>0.01973684210526316</v>
+        <v>0.005793369810106212</v>
       </c>
       <c r="L59">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="M59">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -2577,59 +2529,111 @@
         <v>0</v>
       </c>
       <c r="Q59">
-        <v>447</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="60" spans="10:17">
       <c r="J60" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K60">
-        <v>0.006238859180035651</v>
+        <v>0.005545286506469501</v>
       </c>
       <c r="L60">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="M60">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="N60">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="O60">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="P60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q60">
-        <v>1115</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="61" spans="10:17">
       <c r="J61" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K61">
+        <v>0.005469078670593185</v>
+      </c>
+      <c r="L61">
+        <v>13</v>
+      </c>
+      <c r="M61">
+        <v>15</v>
+      </c>
+      <c r="N61">
+        <v>0.87</v>
+      </c>
+      <c r="O61">
+        <v>0.13</v>
+      </c>
+      <c r="P61" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q61">
+        <v>2364</v>
+      </c>
+    </row>
+    <row r="62" spans="10:17">
+      <c r="J62" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K62">
+        <v>0.004841208365608056</v>
+      </c>
+      <c r="L62">
+        <v>25</v>
+      </c>
+      <c r="M62">
+        <v>26</v>
+      </c>
+      <c r="N62">
+        <v>0.96</v>
+      </c>
+      <c r="O62">
+        <v>0.04000000000000004</v>
+      </c>
+      <c r="P62" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q62">
+        <v>5139</v>
+      </c>
+    </row>
+    <row r="63" spans="10:17">
+      <c r="J63" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K61">
-        <v>0.004009163802978236</v>
-      </c>
-      <c r="L61">
-        <v>7</v>
-      </c>
-      <c r="M61">
-        <v>7</v>
-      </c>
-      <c r="N61">
-        <v>1</v>
-      </c>
-      <c r="O61">
-        <v>0</v>
-      </c>
-      <c r="P61" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q61">
-        <v>1739</v>
+      <c r="K63">
+        <v>0.00420504605526632</v>
+      </c>
+      <c r="L63">
+        <v>21</v>
+      </c>
+      <c r="M63">
+        <v>23</v>
+      </c>
+      <c r="N63">
+        <v>0.91</v>
+      </c>
+      <c r="O63">
+        <v>0.08999999999999997</v>
+      </c>
+      <c r="P63" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q63">
+        <v>4973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>